<commit_message>
tableau de répartition de données
</commit_message>
<xml_diff>
--- a/Documents/tableau_de_données.xlsx
+++ b/Documents/tableau_de_données.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Developpement_Web\Projet H2NCook\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Developpement_Web\Projet_H2NCook\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Dictionnaire de données" sheetId="1" r:id="rId1"/>
     <sheet name="Exemple de données inserées" sheetId="4" r:id="rId2"/>
     <sheet name="Exemple de données de connexion" sheetId="2" r:id="rId3"/>
-    <sheet name="Exemple de d'application" sheetId="3" r:id="rId4"/>
+    <sheet name="Exemple donnéesde d'application" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="289">
   <si>
     <t>Entités</t>
   </si>
@@ -3128,8 +3128,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11:E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6116,26 +6116,1102 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="5" max="5" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="220" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="221"/>
+      <c r="C1" s="221"/>
+      <c r="D1" s="221"/>
+      <c r="E1" s="221"/>
+      <c r="F1" s="221"/>
+      <c r="G1" s="221"/>
+      <c r="H1" s="222"/>
+      <c r="I1" s="108"/>
+      <c r="J1" s="233" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="234"/>
+      <c r="M1" s="220" t="s">
+        <v>15</v>
+      </c>
+      <c r="N1" s="221"/>
+      <c r="O1" s="221"/>
+      <c r="P1" s="221"/>
+      <c r="Q1" s="222"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="120" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="121" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="121" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="121" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" s="121" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="121" t="s">
+        <v>49</v>
+      </c>
+      <c r="G2" s="121" t="s">
+        <v>50</v>
+      </c>
+      <c r="H2" s="122" t="s">
+        <v>51</v>
+      </c>
+      <c r="I2" s="108"/>
+      <c r="J2" s="120" t="s">
+        <v>16</v>
+      </c>
+      <c r="K2" s="122" t="s">
+        <v>17</v>
+      </c>
+      <c r="M2" s="120" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" s="121" t="s">
+        <v>9</v>
+      </c>
+      <c r="O2" s="121" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="121" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="122" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="120">
+        <v>2</v>
+      </c>
+      <c r="B3" s="121" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="121" t="s">
+        <v>177</v>
+      </c>
+      <c r="D3" s="121" t="s">
+        <v>178</v>
+      </c>
+      <c r="E3" s="123">
+        <v>31861.399016203704</v>
+      </c>
+      <c r="F3" s="121" t="s">
+        <v>179</v>
+      </c>
+      <c r="G3" s="121">
+        <v>65421</v>
+      </c>
+      <c r="H3" s="122" t="s">
+        <v>180</v>
+      </c>
+      <c r="I3" s="108"/>
+      <c r="J3" s="120">
+        <v>1</v>
+      </c>
+      <c r="K3" s="122" t="s">
+        <v>263</v>
+      </c>
+      <c r="M3" s="120">
+        <v>1</v>
+      </c>
+      <c r="N3" s="121" t="s">
+        <v>279</v>
+      </c>
+      <c r="O3" s="121" t="s">
+        <v>279</v>
+      </c>
+      <c r="P3" s="121" t="s">
+        <v>280</v>
+      </c>
+      <c r="Q3" s="122">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="124">
+        <v>3</v>
+      </c>
+      <c r="B4" s="125" t="s">
+        <v>181</v>
+      </c>
+      <c r="C4" s="125" t="s">
+        <v>182</v>
+      </c>
+      <c r="D4" s="125" t="s">
+        <v>183</v>
+      </c>
+      <c r="E4" s="126">
+        <v>27651.399016203704</v>
+      </c>
+      <c r="F4" s="125" t="s">
+        <v>184</v>
+      </c>
+      <c r="G4" s="125">
+        <v>71950</v>
+      </c>
+      <c r="H4" s="127" t="s">
+        <v>185</v>
+      </c>
+      <c r="I4" s="108"/>
+      <c r="J4" s="124">
+        <v>2</v>
+      </c>
+      <c r="K4" s="127" t="s">
+        <v>264</v>
+      </c>
+      <c r="M4" s="120">
+        <v>2</v>
+      </c>
+      <c r="N4" s="121" t="s">
+        <v>281</v>
+      </c>
+      <c r="O4" s="121" t="s">
+        <v>281</v>
+      </c>
+      <c r="P4" s="121" t="s">
+        <v>282</v>
+      </c>
+      <c r="Q4" s="122">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M5" s="124">
+        <v>3</v>
+      </c>
+      <c r="N5" s="125" t="s">
+        <v>283</v>
+      </c>
+      <c r="O5" s="125" t="s">
+        <v>283</v>
+      </c>
+      <c r="P5" s="125" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q5" s="127">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="215" t="s">
+        <v>267</v>
+      </c>
+      <c r="B7" s="216"/>
+      <c r="C7" s="216"/>
+      <c r="D7" s="216"/>
+      <c r="E7" s="216"/>
+      <c r="F7" s="217"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="167" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="168" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="168" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="168" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="168" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="169" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="170">
+        <v>1</v>
+      </c>
+      <c r="B9" s="171" t="s">
+        <v>265</v>
+      </c>
+      <c r="C9" s="171">
+        <v>4</v>
+      </c>
+      <c r="D9" s="171" t="s">
+        <v>266</v>
+      </c>
+      <c r="E9" s="172">
+        <v>44280.399016203701</v>
+      </c>
+      <c r="F9" s="173">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="M1:Q1"/>
+    <mergeCell ref="A7:F7"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S20" sqref="S20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="218" t="s">
+        <v>193</v>
+      </c>
+      <c r="B1" s="223"/>
+      <c r="C1" s="223"/>
+      <c r="D1" s="219"/>
+      <c r="G1" s="227" t="s">
+        <v>138</v>
+      </c>
+      <c r="H1" s="228"/>
+      <c r="I1" s="228"/>
+      <c r="J1" s="228"/>
+      <c r="K1" s="228"/>
+      <c r="L1" s="229"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="133" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="140" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" s="140" t="s">
+        <v>192</v>
+      </c>
+      <c r="D2" s="134" t="s">
+        <v>253</v>
+      </c>
+      <c r="G2" s="159" t="s">
+        <v>144</v>
+      </c>
+      <c r="H2" s="160" t="s">
+        <v>131</v>
+      </c>
+      <c r="I2" s="160" t="s">
+        <v>224</v>
+      </c>
+      <c r="J2" s="160" t="s">
+        <v>104</v>
+      </c>
+      <c r="K2" s="160" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" s="161" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="133">
+        <v>1</v>
+      </c>
+      <c r="B3" s="140">
+        <v>1</v>
+      </c>
+      <c r="C3" s="140" t="s">
+        <v>254</v>
+      </c>
+      <c r="D3" s="134">
+        <v>3</v>
+      </c>
+      <c r="G3" s="159">
+        <v>1</v>
+      </c>
+      <c r="H3" s="160">
+        <v>1</v>
+      </c>
+      <c r="I3" s="160">
+        <v>20</v>
+      </c>
+      <c r="J3" s="160" t="s">
+        <v>225</v>
+      </c>
+      <c r="K3" s="160">
+        <v>1</v>
+      </c>
+      <c r="L3" s="161">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="133">
+        <v>2</v>
+      </c>
+      <c r="B4" s="140">
+        <v>1</v>
+      </c>
+      <c r="C4" s="140" t="s">
+        <v>255</v>
+      </c>
+      <c r="D4" s="134">
+        <v>4</v>
+      </c>
+      <c r="G4" s="159">
+        <v>2</v>
+      </c>
+      <c r="H4" s="160">
+        <v>1</v>
+      </c>
+      <c r="I4" s="160">
+        <v>20</v>
+      </c>
+      <c r="J4" s="160">
+        <v>12</v>
+      </c>
+      <c r="K4" s="160" t="s">
+        <v>225</v>
+      </c>
+      <c r="L4" s="161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="133">
+        <v>3</v>
+      </c>
+      <c r="B5" s="140">
+        <v>1</v>
+      </c>
+      <c r="C5" s="140" t="s">
+        <v>256</v>
+      </c>
+      <c r="D5" s="134">
+        <v>2</v>
+      </c>
+      <c r="G5" s="162">
+        <v>3</v>
+      </c>
+      <c r="H5" s="163">
+        <v>1</v>
+      </c>
+      <c r="I5" s="163" t="s">
+        <v>226</v>
+      </c>
+      <c r="J5" s="163">
+        <v>12</v>
+      </c>
+      <c r="K5" s="163" t="s">
+        <v>225</v>
+      </c>
+      <c r="L5" s="164">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="133">
+        <v>4</v>
+      </c>
+      <c r="B6" s="140">
+        <v>1</v>
+      </c>
+      <c r="C6" s="140" t="s">
+        <v>257</v>
+      </c>
+      <c r="D6" s="134">
+        <v>5</v>
+      </c>
+      <c r="O6" s="218" t="s">
+        <v>175</v>
+      </c>
+      <c r="P6" s="219"/>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="133">
+        <v>5</v>
+      </c>
+      <c r="B7" s="140">
+        <v>3</v>
+      </c>
+      <c r="C7" s="140">
+        <v>10</v>
+      </c>
+      <c r="D7" s="134">
+        <v>1</v>
+      </c>
+      <c r="O7" s="133" t="s">
+        <v>116</v>
+      </c>
+      <c r="P7" s="134" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="133">
+        <v>6</v>
+      </c>
+      <c r="B8" s="140">
+        <v>3</v>
+      </c>
+      <c r="C8" s="140" t="s">
+        <v>254</v>
+      </c>
+      <c r="D8" s="134">
+        <v>4</v>
+      </c>
+      <c r="G8" s="227" t="s">
+        <v>186</v>
+      </c>
+      <c r="H8" s="228"/>
+      <c r="I8" s="228"/>
+      <c r="J8" s="228"/>
+      <c r="K8" s="229"/>
+      <c r="O8" s="133">
+        <v>1</v>
+      </c>
+      <c r="P8" s="134" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="133">
+        <v>7</v>
+      </c>
+      <c r="B9" s="140">
+        <v>3</v>
+      </c>
+      <c r="C9" s="140" t="s">
+        <v>255</v>
+      </c>
+      <c r="D9" s="134">
+        <v>2</v>
+      </c>
+      <c r="G9" s="128" t="s">
+        <v>150</v>
+      </c>
+      <c r="H9" s="129" t="s">
+        <v>151</v>
+      </c>
+      <c r="I9" s="129" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" s="129" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="130" t="s">
+        <v>77</v>
+      </c>
+      <c r="O9" s="133">
+        <v>2</v>
+      </c>
+      <c r="P9" s="134" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="133">
+        <v>8</v>
+      </c>
+      <c r="B10" s="140">
+        <v>3</v>
+      </c>
+      <c r="C10" s="140" t="s">
+        <v>258</v>
+      </c>
+      <c r="D10" s="134">
+        <v>5</v>
+      </c>
+      <c r="G10" s="128">
+        <v>1</v>
+      </c>
+      <c r="H10" s="129">
+        <v>2151357</v>
+      </c>
+      <c r="I10" s="129">
+        <v>2</v>
+      </c>
+      <c r="J10" s="129">
+        <v>1</v>
+      </c>
+      <c r="K10" s="130">
+        <v>1</v>
+      </c>
+      <c r="O10" s="133">
+        <v>3</v>
+      </c>
+      <c r="P10" s="134" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="133">
+        <v>9</v>
+      </c>
+      <c r="B11" s="140">
+        <v>4</v>
+      </c>
+      <c r="C11" s="140">
+        <v>100</v>
+      </c>
+      <c r="D11" s="134">
+        <v>1</v>
+      </c>
+      <c r="G11" s="135">
+        <v>2</v>
+      </c>
+      <c r="H11" s="136">
+        <v>2659892</v>
+      </c>
+      <c r="I11" s="136">
+        <v>3</v>
+      </c>
+      <c r="J11" s="136">
+        <v>2</v>
+      </c>
+      <c r="K11" s="137">
+        <v>2</v>
+      </c>
+      <c r="O11" s="138">
+        <v>4</v>
+      </c>
+      <c r="P11" s="139" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="133">
+        <v>10</v>
+      </c>
+      <c r="B12" s="140">
+        <v>4</v>
+      </c>
+      <c r="C12" s="140">
+        <v>10</v>
+      </c>
+      <c r="D12" s="134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="133">
+        <v>11</v>
+      </c>
+      <c r="B13" s="140">
+        <v>4</v>
+      </c>
+      <c r="C13" s="140" t="s">
+        <v>254</v>
+      </c>
+      <c r="D13" s="134">
+        <v>2</v>
+      </c>
+      <c r="J13" s="218" t="s">
+        <v>117</v>
+      </c>
+      <c r="K13" s="223"/>
+      <c r="L13" s="223"/>
+      <c r="M13" s="223"/>
+      <c r="N13" s="223"/>
+      <c r="O13" s="219"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="133">
+        <v>12</v>
+      </c>
+      <c r="B14" s="140">
+        <v>4</v>
+      </c>
+      <c r="C14" s="140" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="134">
+        <v>5</v>
+      </c>
+      <c r="J14" s="133" t="s">
+        <v>123</v>
+      </c>
+      <c r="K14" s="140" t="s">
+        <v>17</v>
+      </c>
+      <c r="L14" s="140" t="s">
+        <v>119</v>
+      </c>
+      <c r="M14" s="140" t="s">
+        <v>120</v>
+      </c>
+      <c r="N14" s="140" t="s">
+        <v>122</v>
+      </c>
+      <c r="O14" s="134" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="133">
+        <v>13</v>
+      </c>
+      <c r="B15" s="140">
+        <v>2</v>
+      </c>
+      <c r="C15" s="140">
+        <v>1000</v>
+      </c>
+      <c r="D15" s="134">
+        <v>1</v>
+      </c>
+      <c r="J15" s="138">
+        <v>1</v>
+      </c>
+      <c r="K15" s="143" t="s">
+        <v>249</v>
+      </c>
+      <c r="L15" s="143">
+        <v>1</v>
+      </c>
+      <c r="M15" s="143" t="s">
+        <v>250</v>
+      </c>
+      <c r="N15" s="143" t="s">
+        <v>251</v>
+      </c>
+      <c r="O15" s="139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="133">
+        <v>14</v>
+      </c>
+      <c r="B16" s="140">
+        <v>2</v>
+      </c>
+      <c r="C16" s="140">
+        <v>100</v>
+      </c>
+      <c r="D16" s="134">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="133">
+        <v>15</v>
+      </c>
+      <c r="B17" s="140">
+        <v>2</v>
+      </c>
+      <c r="C17" s="140">
+        <v>10</v>
+      </c>
+      <c r="D17" s="134">
+        <v>4</v>
+      </c>
+      <c r="G17" s="218" t="s">
+        <v>208</v>
+      </c>
+      <c r="H17" s="223"/>
+      <c r="I17" s="223"/>
+      <c r="J17" s="219"/>
+      <c r="L17" s="218" t="s">
+        <v>205</v>
+      </c>
+      <c r="M17" s="223"/>
+      <c r="N17" s="219"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A18" s="133">
+        <v>16</v>
+      </c>
+      <c r="B18" s="140">
+        <v>2</v>
+      </c>
+      <c r="C18" s="140" t="s">
+        <v>256</v>
+      </c>
+      <c r="D18" s="134">
+        <v>5</v>
+      </c>
+      <c r="G18" s="153" t="s">
+        <v>206</v>
+      </c>
+      <c r="H18" s="154" t="s">
+        <v>207</v>
+      </c>
+      <c r="I18" s="154" t="s">
+        <v>123</v>
+      </c>
+      <c r="J18" s="155" t="s">
+        <v>195</v>
+      </c>
+      <c r="L18" s="133" t="s">
+        <v>195</v>
+      </c>
+      <c r="M18" s="140" t="s">
+        <v>25</v>
+      </c>
+      <c r="N18" s="134" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A19" s="133">
+        <v>17</v>
+      </c>
+      <c r="B19" s="140">
+        <v>5</v>
+      </c>
+      <c r="C19" s="140">
+        <v>1000000</v>
+      </c>
+      <c r="D19" s="134">
+        <v>1</v>
+      </c>
+      <c r="G19" s="133">
+        <v>1</v>
+      </c>
+      <c r="H19" s="140">
+        <v>1</v>
+      </c>
+      <c r="I19" s="140">
+        <v>1</v>
+      </c>
+      <c r="J19" s="134">
+        <v>1</v>
+      </c>
+      <c r="L19" s="133">
+        <v>1</v>
+      </c>
+      <c r="M19" s="140" t="s">
+        <v>197</v>
+      </c>
+      <c r="N19" s="134" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" s="133">
+        <v>18</v>
+      </c>
+      <c r="B20" s="140">
+        <v>5</v>
+      </c>
+      <c r="C20" s="140">
+        <v>100000</v>
+      </c>
+      <c r="D20" s="134">
+        <v>3</v>
+      </c>
+      <c r="G20" s="133">
+        <v>2</v>
+      </c>
+      <c r="H20" s="140">
+        <v>2</v>
+      </c>
+      <c r="I20" s="140">
+        <v>1</v>
+      </c>
+      <c r="J20" s="134">
+        <v>2</v>
+      </c>
+      <c r="L20" s="133">
+        <v>2</v>
+      </c>
+      <c r="M20" s="140" t="s">
+        <v>199</v>
+      </c>
+      <c r="N20" s="134" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A21" s="133">
+        <v>19</v>
+      </c>
+      <c r="B21" s="140">
+        <v>5</v>
+      </c>
+      <c r="C21" s="140">
+        <v>10000</v>
+      </c>
+      <c r="D21" s="134">
+        <v>4</v>
+      </c>
+      <c r="G21" s="133">
+        <v>3</v>
+      </c>
+      <c r="H21" s="140">
+        <v>3</v>
+      </c>
+      <c r="I21" s="140">
+        <v>1</v>
+      </c>
+      <c r="J21" s="134">
+        <v>3</v>
+      </c>
+      <c r="L21" s="133">
+        <v>3</v>
+      </c>
+      <c r="M21" s="140" t="s">
+        <v>201</v>
+      </c>
+      <c r="N21" s="134" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="133">
+        <v>20</v>
+      </c>
+      <c r="B22" s="140">
+        <v>5</v>
+      </c>
+      <c r="C22" s="140">
+        <v>1000</v>
+      </c>
+      <c r="D22" s="134">
+        <v>2</v>
+      </c>
+      <c r="G22" s="138">
+        <v>4</v>
+      </c>
+      <c r="H22" s="143">
+        <v>4</v>
+      </c>
+      <c r="I22" s="143">
+        <v>1</v>
+      </c>
+      <c r="J22" s="139">
+        <v>4</v>
+      </c>
+      <c r="L22" s="138">
+        <v>4</v>
+      </c>
+      <c r="M22" s="143" t="s">
+        <v>203</v>
+      </c>
+      <c r="N22" s="139" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A23" s="133">
+        <v>21</v>
+      </c>
+      <c r="B23" s="140">
+        <v>7</v>
+      </c>
+      <c r="C23" s="140" t="s">
+        <v>254</v>
+      </c>
+      <c r="D23" s="134">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A24" s="133">
+        <v>22</v>
+      </c>
+      <c r="B24" s="140">
+        <v>7</v>
+      </c>
+      <c r="C24" s="140" t="s">
+        <v>255</v>
+      </c>
+      <c r="D24" s="134">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A25" s="133">
+        <v>23</v>
+      </c>
+      <c r="B25" s="140">
+        <v>7</v>
+      </c>
+      <c r="C25" s="140" t="s">
+        <v>256</v>
+      </c>
+      <c r="D25" s="134">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A26" s="133">
+        <v>24</v>
+      </c>
+      <c r="B26" s="140">
+        <v>7</v>
+      </c>
+      <c r="C26" s="140" t="s">
+        <v>257</v>
+      </c>
+      <c r="D26" s="134">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="138">
+        <v>25</v>
+      </c>
+      <c r="B27" s="143">
+        <v>8</v>
+      </c>
+      <c r="C27" s="143">
+        <v>10</v>
+      </c>
+      <c r="D27" s="139">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G28" s="218" t="s">
+        <v>278</v>
+      </c>
+      <c r="H28" s="219"/>
+      <c r="K28" s="218" t="s">
+        <v>135</v>
+      </c>
+      <c r="L28" s="223"/>
+      <c r="M28" s="219"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G29" s="133" t="s">
+        <v>187</v>
+      </c>
+      <c r="H29" s="134" t="s">
+        <v>17</v>
+      </c>
+      <c r="K29" s="133" t="s">
+        <v>137</v>
+      </c>
+      <c r="L29" s="140" t="s">
+        <v>17</v>
+      </c>
+      <c r="M29" s="134" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G30" s="133">
+        <v>1</v>
+      </c>
+      <c r="H30" s="134" t="s">
+        <v>268</v>
+      </c>
+      <c r="K30" s="138">
+        <v>1</v>
+      </c>
+      <c r="L30" s="143" t="s">
+        <v>231</v>
+      </c>
+      <c r="M30" s="139">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G31" s="133">
+        <v>2</v>
+      </c>
+      <c r="H31" s="134" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G32" s="133">
+        <v>3</v>
+      </c>
+      <c r="H32" s="134" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="33" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G33" s="133">
+        <v>4</v>
+      </c>
+      <c r="H33" s="134" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="34" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G34" s="133">
+        <v>5</v>
+      </c>
+      <c r="H34" s="134" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="35" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G35" s="133">
+        <v>6</v>
+      </c>
+      <c r="H35" s="134" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="36" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G36" s="133">
+        <v>7</v>
+      </c>
+      <c r="H36" s="134" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="37" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G37" s="133">
+        <v>8</v>
+      </c>
+      <c r="H37" s="134" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="38" spans="7:8" x14ac:dyDescent="0.25">
+      <c r="G38" s="133">
+        <v>9</v>
+      </c>
+      <c r="H38" s="134" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="39" spans="7:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="G39" s="138">
+        <v>10</v>
+      </c>
+      <c r="H39" s="139" t="s">
+        <v>277</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="G8:K8"/>
+    <mergeCell ref="G17:J17"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="G28:H28"/>
+    <mergeCell ref="K28:M28"/>
+    <mergeCell ref="J13:O13"/>
+    <mergeCell ref="O6:P6"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>